<commit_message>
completed the experiment 2 readings
</commit_message>
<xml_diff>
--- a/menimgUrl.xlsx
+++ b/menimgUrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\skyarup\TobbiSwiping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC21A6CF-DFB8-4F7B-8801-5CF8DD954FE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B1477-2859-463F-9EA0-FCD5438A7E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13170" xr2:uid="{EC64C2F6-AAEA-4317-BC51-9C7CBF0D9778}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13170" xr2:uid="{8FDA86ED-7987-41A8-B38B-CE9B64405113}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Original</t>
   </si>
@@ -33,184 +33,208 @@
     <t>Scramble</t>
   </si>
   <si>
-    <t>men/1-original.jpg</t>
-  </si>
-  <si>
-    <t>men/1-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/10-original.jpg</t>
-  </si>
-  <si>
-    <t>men/10-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/11-original.jpg</t>
-  </si>
-  <si>
-    <t>men/11-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/12-original.jpg</t>
-  </si>
-  <si>
-    <t>men/12-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/13-original.jpg</t>
-  </si>
-  <si>
-    <t>men/13-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/14-original.jpg</t>
-  </si>
-  <si>
-    <t>men/14-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/15-original.jpg</t>
-  </si>
-  <si>
-    <t>men/15-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/16-original.jpg</t>
-  </si>
-  <si>
-    <t>men/16-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/17-original.jpg</t>
-  </si>
-  <si>
-    <t>men/17-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/18-original.jpg</t>
-  </si>
-  <si>
-    <t>men/18-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/19-original.jpg</t>
-  </si>
-  <si>
-    <t>men/19-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/2-original.jpg</t>
-  </si>
-  <si>
-    <t>men/2-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/20-original.jpg</t>
-  </si>
-  <si>
-    <t>men/20-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/21-original.jpg</t>
-  </si>
-  <si>
-    <t>men/21-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/22-original.jpg</t>
-  </si>
-  <si>
-    <t>men/22-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/23-original.jpg</t>
-  </si>
-  <si>
-    <t>men/23-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/24-original.jpg</t>
-  </si>
-  <si>
-    <t>men/24-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/25-original.jpg</t>
-  </si>
-  <si>
-    <t>men/25-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/26-original.jpg</t>
-  </si>
-  <si>
-    <t>men/26-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/27-original.jpg</t>
-  </si>
-  <si>
-    <t>men/27-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/28-original.jpg</t>
-  </si>
-  <si>
-    <t>men/28-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/29-original.jpg</t>
-  </si>
-  <si>
-    <t>men/29-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/3-original.jpg</t>
-  </si>
-  <si>
-    <t>men/3-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/30-original.jpg</t>
-  </si>
-  <si>
-    <t>men/30-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/4-original.jpg</t>
-  </si>
-  <si>
-    <t>men/4-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/5-original.jpg</t>
-  </si>
-  <si>
-    <t>men/5-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/6-original.jpg</t>
-  </si>
-  <si>
-    <t>men/6-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/7-original.jpg</t>
-  </si>
-  <si>
-    <t>men/7-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/8-original.jpg</t>
-  </si>
-  <si>
-    <t>men/8-scramble.jpg</t>
-  </si>
-  <si>
-    <t>men/9-original.jpg</t>
-  </si>
-  <si>
-    <t>men/9-scramble.jpg</t>
+    <t>men1/1-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/1-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/10-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/10-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/11-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/11-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/12-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/12-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/13-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/13-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/14-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/14-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/15-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/15-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/16-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/16-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/17-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/17-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/18-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/18-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/19-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/19-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/2-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/2-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/20-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/20-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/21-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/21-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/22-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/22-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/23-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/23-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/24-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/24-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/25-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/25-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/26-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/26-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/27-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/27-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/28-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/28-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/29-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/29-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/3-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/3-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/30-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/30-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/31-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/31-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/32-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/32-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/33-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/33-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/34-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/34-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/4-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/4-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/5-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/5-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/6-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/6-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/7-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/7-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/8-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/8-scramble.jpg</t>
+  </si>
+  <si>
+    <t>men1/9-original.jpg</t>
+  </si>
+  <si>
+    <t>men1/9-scramble.jpg</t>
   </si>
 </sst>
 </file>
@@ -561,14 +585,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0342BB-55E3-4CF1-A908-8BC32419F211}">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718F273-89CF-4E22-8720-94CD7BA3ABD5}">
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A2" sqref="A2:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -818,6 +846,38 @@
         <v>61</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>